<commit_message>
Complete except for Q1
</commit_message>
<xml_diff>
--- a/hw5/calcs.xlsx
+++ b/hw5/calcs.xlsx
@@ -20,85 +20,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>p(1)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>p(2)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>p(3)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>End</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>∑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Q</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>End</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>F</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>F</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitterbi</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum of all Paths:</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>End (p=.25)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Forward (D1, x=4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backwards (5-&gt;End):</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vitterbi log</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="10">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -106,14 +126,21 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.00000000"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
+    <numFmt numFmtId="172" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -130,7 +157,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,17 +165,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,20 +525,119 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B6:O12"/>
+  <dimension ref="B2:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.5703125" defaultRowHeight="23" customHeight="1"/>
   <cols>
-    <col min="9" max="13" width="11.5703125" customWidth="1"/>
+    <col min="9" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
     <col min="14" max="14" width="12.140625" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:15" ht="23" customHeight="1">
+    <row r="2" spans="2:16" ht="23" customHeight="1">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" ht="23" customHeight="1">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="2">
+        <f>LOG(0.5*0.5,2)</f>
+        <v>-2</v>
+      </c>
+      <c r="J3" s="2">
+        <f>MAX(LOG(0.5,2)+I$3+LOG(VLOOKUP($H$3,$B$6:$E$8,J$6+1),2),LOG(0.25,2)+I$4+LOG(VLOOKUP($H$3,$B$6:$E$8,J$6+1),2))</f>
+        <v>-4</v>
+      </c>
+      <c r="K3" s="2">
+        <f t="shared" ref="K3:N3" si="0">MAX(LOG(0.5,2)+J$3+LOG(VLOOKUP($H$3,$B$6:$E$8,K$6+1),2),LOG(0.25,2)+J$4+LOG(VLOOKUP($H$3,$B$6:$E$8,K$6+1),2))</f>
+        <v>-7</v>
+      </c>
+      <c r="L3" s="2">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="M3" s="2">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="N3" s="2">
+        <f t="shared" si="0"/>
+        <v>-15</v>
+      </c>
+      <c r="O3" s="4">
+        <f>N3+LOG(0.25,2)</f>
+        <v>-17</v>
+      </c>
+      <c r="P3" s="7"/>
+    </row>
+    <row r="4" spans="2:16" ht="23" customHeight="1">
+      <c r="H4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3">
+        <f>LOG(0.5*0.25,2)</f>
+        <v>-3</v>
+      </c>
+      <c r="J4" s="3">
+        <f>MAX(LOG(0.25,2)+I$3+LOG(VLOOKUP($H$4,$B$6:$E$8,J$6+1),2),LOG(0.5,2)+I$4+LOG(VLOOKUP($H$4,$B$6:$E$8,J$6+1),2))</f>
+        <v>-6</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:N4" si="1">MAX(LOG(0.25,2)+J$3+LOG(VLOOKUP($H$4,$B$6:$E$8,K$6+1),2),LOG(0.5,2)+J$4+LOG(VLOOKUP($H$4,$B$6:$E$8,K$6+1),2))</f>
+        <v>-7</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="N4" s="3">
+        <f t="shared" si="1"/>
+        <v>-14</v>
+      </c>
+      <c r="O4" s="2">
+        <f>N4+LOG(0.25,2)</f>
+        <v>-16</v>
+      </c>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="2:16" ht="23" customHeight="1">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="23" customHeight="1">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -524,10 +669,10 @@
         <v>2</v>
       </c>
       <c r="O6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" ht="23" customHeight="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="23" customHeight="1">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -548,31 +693,31 @@
         <v>0.25</v>
       </c>
       <c r="J7" s="2">
-        <f>MAX(0.5*I$7*VLOOKUP($H$7,$B$6:$E$8,J$6+1),0.25*I$8*VLOOKUP($H$8,$B$6:$E$8,J$6+1))</f>
+        <f>MAX(0.5*I$7*VLOOKUP($H$7,$B$6:$E$8,J$6+1),0.25*I$8*VLOOKUP($H$7,$B$6:$E$8,J$6+1))</f>
         <v>6.25E-2</v>
       </c>
-      <c r="K7" s="3">
-        <f t="shared" ref="K7:N7" si="0">MAX(0.5*J$7*VLOOKUP($H$7,$B$6:$E$8,K$6+1),0.25*J$8*VLOOKUP($H$8,$B$6:$E$8,K$6+1))</f>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:N7" si="2">MAX(0.5*J$7*VLOOKUP($H$7,$B$6:$E$8,K$6+1),0.25*J$8*VLOOKUP($H$7,$B$6:$E$8,K$6+1))</f>
         <v>7.8125E-3</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.953125E-3</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.44140625E-4</v>
       </c>
-      <c r="N7" s="3">
-        <f t="shared" si="0"/>
+      <c r="N7" s="4">
+        <f t="shared" si="2"/>
         <v>3.0517578125E-5</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="4">
         <f>N7*0.25</f>
         <v>7.62939453125E-6</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="23" customHeight="1">
+    <row r="8" spans="2:16" ht="23" customHeight="1">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -593,36 +738,36 @@
         <v>0.125</v>
       </c>
       <c r="J8" s="3">
-        <f>MAX(0.25*I$7*VLOOKUP($H$7,$B$6:$E$8,J$6+1),0.5*I$8*VLOOKUP($H$8,$B$6:$E$8,J$6+1))</f>
-        <v>3.125E-2</v>
-      </c>
-      <c r="K8" s="3">
-        <f t="shared" ref="K8:N8" si="1">MAX(0.25*J$7*VLOOKUP($H$7,$B$6:$E$8,K$6+1),0.5*J$8*VLOOKUP($H$8,$B$6:$E$8,K$6+1))</f>
+        <f>MAX(0.25*I$7*VLOOKUP($H$8,$B$6:$E$8,J$6+1),0.5*I$8*VLOOKUP($H$8,$B$6:$E$8,J$6+1))</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" ref="K8:N8" si="3">MAX(0.25*J$7*VLOOKUP($H$8,$B$6:$E$8,K$6+1),0.5*J$8*VLOOKUP($H$8,$B$6:$E$8,K$6+1))</f>
         <v>7.8125E-3</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.765625E-4</v>
       </c>
-      <c r="M8" s="3">
-        <f t="shared" si="1"/>
+      <c r="M8" s="2">
+        <f t="shared" si="3"/>
         <v>2.44140625E-4</v>
       </c>
       <c r="N8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.103515625E-5</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="2">
         <f>N8*0.25</f>
         <v>1.52587890625E-5</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="23" customHeight="1">
+    <row r="9" spans="2:16" ht="23" customHeight="1">
       <c r="H9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" ht="23" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="23" customHeight="1">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -636,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="23" customHeight="1">
+    <row r="11" spans="2:16" ht="23" customHeight="1">
       <c r="B11" t="s">
         <v>3</v>
       </c>
@@ -649,8 +794,29 @@
       <c r="E11">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" ht="23" customHeight="1">
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" ht="23" customHeight="1">
       <c r="B12" t="s">
         <v>4</v>
       </c>
@@ -663,11 +829,193 @@
       <c r="E12">
         <v>0.25</v>
       </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="4">
+        <f>0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="4">
+        <f>SUM(0.5*I$12*VLOOKUP($H$7,$B$6:$E$8,J$6+1),0.25*I$13*VLOOKUP($H$7,$B$6:$E$8,J$6+1))</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="K12" s="4">
+        <f t="shared" ref="K12:N12" si="4">SUM(0.5*J$12*VLOOKUP($H$7,$B$6:$E$8,K$6+1),0.25*J$13*VLOOKUP($H$7,$B$6:$E$8,K$6+1))</f>
+        <v>1.171875E-2</v>
+      </c>
+      <c r="L12" s="4">
+        <f t="shared" si="4"/>
+        <v>5.126953125E-3</v>
+      </c>
+      <c r="M12" s="4">
+        <f t="shared" si="4"/>
+        <v>8.23974609375E-4</v>
+      </c>
+      <c r="N12" s="4">
+        <f t="shared" si="4"/>
+        <v>1.888275146484375E-4</v>
+      </c>
+      <c r="O12" s="4">
+        <f>N12*0.25</f>
+        <v>4.7206878662109375E-5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" ht="23" customHeight="1">
+      <c r="H13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="4">
+        <f>0.5*0.25</f>
+        <v>0.125</v>
+      </c>
+      <c r="J13" s="4">
+        <f>SUM(0.25*I$12*VLOOKUP($H$8,$B$6:$E$8,J$6+1),0.5*I$13*VLOOKUP($H$8,$B$6:$E$8,J$6+1))</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" ref="K13:N13" si="5">SUM(0.25*J$12*VLOOKUP($H$8,$B$6:$E$8,K$6+1),0.5*J$13*VLOOKUP($H$8,$B$6:$E$8,K$6+1))</f>
+        <v>1.7578125E-2</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="5"/>
+        <v>2.9296875E-3</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="5"/>
+        <v>1.373291015625E-3</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="5"/>
+        <v>4.46319580078125E-4</v>
+      </c>
+      <c r="O13" s="4">
+        <f>N13*0.25</f>
+        <v>1.1157989501953125E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" ht="23" customHeight="1">
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="6">
+        <f>L12</f>
+        <v>5.126953125E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" ht="23" customHeight="1">
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15" ht="23" customHeight="1">
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="2">
+        <f>0.5*0.5</f>
+        <v>0.25</v>
+      </c>
+      <c r="J17" s="2">
+        <f>SUM(0.5*I$12*VLOOKUP($H$7,$B$6:$E$8,J$6+1),0.25*I$13*VLOOKUP($H$7,$B$6:$E$8,J$6+1))</f>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" ref="K17:N17" si="6">SUM(0.5*J$12*VLOOKUP($H$7,$B$6:$E$8,K$6+1),0.25*J$13*VLOOKUP($H$7,$B$6:$E$8,K$6+1))</f>
+        <v>1.171875E-2</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1</v>
+      </c>
+      <c r="M17" s="2">
+        <f>SUM(0.5*L$17*VLOOKUP($H$7,$B$6:$E$8,M$6+1),0.25*L$18*VLOOKUP($H$7,$B$6:$E$8,M$6+1))</f>
+        <v>0.125</v>
+      </c>
+      <c r="N17" s="2">
+        <f>SUM(0.5*M$17*VLOOKUP($H$7,$B$6:$E$8,N$6+1),0.25*M$18*VLOOKUP($H$7,$B$6:$E$8,N$6+1))</f>
+        <v>2.34375E-2</v>
+      </c>
+      <c r="O17" s="4">
+        <f>N17*0.25</f>
+        <v>5.859375E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" ht="23" customHeight="1">
+      <c r="H18" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <f>0.5*0.25</f>
+        <v>0.125</v>
+      </c>
+      <c r="J18" s="3">
+        <f>SUM(0.25*I$12*VLOOKUP($H$8,$B$6:$E$8,J$6+1),0.5*I$13*VLOOKUP($H$8,$B$6:$E$8,J$6+1))</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ref="K18:N18" si="7">SUM(0.25*J$12*VLOOKUP($H$8,$B$6:$E$8,K$6+1),0.5*J$13*VLOOKUP($H$8,$B$6:$E$8,K$6+1))</f>
+        <v>1.7578125E-2</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <f>SUM(0.25*L$17*VLOOKUP($H$8,$B$6:$E$8,M$6+1),0.5*L$18*VLOOKUP($H$8,$B$6:$E$8,M$6+1))</f>
+        <v>0.125</v>
+      </c>
+      <c r="N18" s="3">
+        <f>SUM(0.25*M$17*VLOOKUP($H$8,$B$6:$E$8,N$6+1),0.5*M$18*VLOOKUP($H$8,$B$6:$E$8,N$6+1))</f>
+        <v>4.6875E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <f>N18*0.25</f>
+        <v>1.171875E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15" ht="23" customHeight="1">
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="6">
+        <f>SUM(O17:O18)</f>
+        <v>1.7578125E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15" ht="23" customHeight="1">
+      <c r="L20" s="5"/>
+    </row>
+    <row r="22" spans="8:15" ht="23" customHeight="1">
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="6">
+        <f>SUM(O12:O13)</f>
+        <v>1.5878677368164062E-4</v>
+      </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -692,27 +1040,27 @@
   <sheetData>
     <row r="2" spans="2:8" ht="21" customHeight="1">
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="21" customHeight="1">
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>
@@ -735,7 +1083,7 @@
     </row>
     <row r="4" spans="2:8" ht="21" customHeight="1">
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>18</v>
@@ -758,7 +1106,7 @@
     </row>
     <row r="5" spans="2:8" ht="21" customHeight="1">
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1">
         <v>15</v>
@@ -781,7 +1129,7 @@
     </row>
     <row r="6" spans="2:8" ht="21" customHeight="1">
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="1">
         <v>21</v>
@@ -804,7 +1152,7 @@
     </row>
     <row r="7" spans="2:8" ht="21" customHeight="1">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1">
         <v>6</v>
@@ -827,7 +1175,7 @@
     </row>
     <row r="8" spans="2:8" ht="21" customHeight="1">
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>16</v>
@@ -850,7 +1198,7 @@
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>